<commit_message>
Refactored code. Percolation.c is now main.c
</commit_message>
<xml_diff>
--- a/execution-time-charts.xlsx
+++ b/execution-time-charts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="600" windowWidth="19300" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="3360" yWindow="460" windowWidth="25440" windowHeight="15320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Size</t>
   </si>
@@ -53,24 +53,6 @@
     <t>T: Total</t>
   </si>
   <si>
-    <t>Peroclates?</t>
-  </si>
-  <si>
-    <t>Cluster size</t>
-  </si>
-  <si>
-    <t>SUCCEEDED</t>
-  </si>
-  <si>
-    <t>FAILED</t>
-  </si>
-  <si>
-    <t>Thu Jan  1 08:00:00 1970</t>
-  </si>
-  <si>
-    <t>Lattice</t>
-  </si>
-  <si>
     <t>Site</t>
   </si>
   <si>
@@ -81,6 +63,12 @@
   </si>
   <si>
     <t>Threads</t>
+  </si>
+  <si>
+    <t>Runs</t>
+  </si>
+  <si>
+    <t>Wed Oct  4 16:38:37 2017</t>
   </si>
 </sst>
 </file>
@@ -217,7 +205,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$6</c:f>
+              <c:f>Sheet1!$C$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -252,10 +240,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$18</c:f>
+              <c:f>Sheet1!$A$8:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>16.0</c:v>
                 </c:pt>
@@ -285,57 +273,45 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>8192.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16384.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>32768.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$18</c:f>
+              <c:f>Sheet1!$C$8:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0.035694</c:v>
+                  <c:v>0.018115</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.042312</c:v>
+                  <c:v>0.091719</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.316508</c:v>
+                  <c:v>0.227781</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.276789</c:v>
+                  <c:v>0.539342</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.46348</c:v>
+                  <c:v>1.745716</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.998203</c:v>
+                  <c:v>7.539005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.627318</c:v>
+                  <c:v>30.83874</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80.662372</c:v>
+                  <c:v>104.765969</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>184.232116</c:v>
+                  <c:v>228.423695</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>834.250049</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1696.432703</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3594.287048</c:v>
+                  <c:v>718.459334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -347,7 +323,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$6</c:f>
+              <c:f>Sheet1!$D$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -382,10 +358,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$18</c:f>
+              <c:f>Sheet1!$A$8:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>16.0</c:v>
                 </c:pt>
@@ -415,57 +391,45 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>8192.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16384.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>32768.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$18</c:f>
+              <c:f>Sheet1!$D$8:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0.128893</c:v>
+                  <c:v>0.110529</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.086396</c:v>
+                  <c:v>0.123476</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.31264</c:v>
+                  <c:v>0.209851</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.313181</c:v>
+                  <c:v>0.531094</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.925725</c:v>
+                  <c:v>1.996095</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.172279</c:v>
+                  <c:v>11.299107</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.221877</c:v>
+                  <c:v>77.448294</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>75.349418</c:v>
+                  <c:v>301.092592</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80.16945200000001</c:v>
+                  <c:v>170.827136</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>687.683842</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1174.439164</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2985.523488</c:v>
+                  <c:v>517.917639</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -480,11 +444,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1594662032"/>
-        <c:axId val="1594312480"/>
+        <c:axId val="1655770192"/>
+        <c:axId val="1655772320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1594662032"/>
+        <c:axId val="1655770192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -596,12 +560,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1594312480"/>
+        <c:crossAx val="1655772320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1594312480"/>
+        <c:axId val="1655772320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -719,7 +683,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1594662032"/>
+        <c:crossAx val="1655770192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -886,7 +850,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$6</c:f>
+              <c:f>Sheet1!$G$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -921,10 +885,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$18</c:f>
+              <c:f>Sheet1!$A$8:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>16.0</c:v>
                 </c:pt>
@@ -954,57 +918,45 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>8192.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16384.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>32768.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$7:$G$18</c:f>
+              <c:f>Sheet1!$G$8:$G$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0.047365</c:v>
+                  <c:v>0.029833</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.084967</c:v>
+                  <c:v>0.1343</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.499809</c:v>
+                  <c:v>0.372702</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.875417</c:v>
+                  <c:v>1.129693</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.755554</c:v>
+                  <c:v>3.820088</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.82783</c:v>
+                  <c:v>15.729909</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>63.287739</c:v>
+                  <c:v>65.30939600000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>222.13024</c:v>
+                  <c:v>245.204265</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>745.656306</c:v>
+                  <c:v>821.55439</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3096.624539</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11036.03871</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>44009.04582</c:v>
+                  <c:v>3139.762408</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1016,7 +968,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$6</c:f>
+              <c:f>Sheet1!$H$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1051,10 +1003,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$18</c:f>
+              <c:f>Sheet1!$A$8:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>16.0</c:v>
                 </c:pt>
@@ -1084,57 +1036,45 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>8192.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16384.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>32768.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$7:$H$18</c:f>
+              <c:f>Sheet1!$H$8:$H$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0.128893</c:v>
+                  <c:v>0.122247</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.086396</c:v>
+                  <c:v>0.166057</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.31264</c:v>
+                  <c:v>0.354772</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.313181</c:v>
+                  <c:v>1.121445</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.925725</c:v>
+                  <c:v>4.070466</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.172279</c:v>
+                  <c:v>19.490011</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.221877</c:v>
+                  <c:v>111.918951</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>75.349418</c:v>
+                  <c:v>441.530889</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80.16945200000001</c:v>
+                  <c:v>763.9578310000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>687.683842</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1174.439164</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2985.523488</c:v>
+                  <c:v>2939.220713</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1149,11 +1089,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1625667264"/>
-        <c:axId val="1600031648"/>
+        <c:axId val="1598816496"/>
+        <c:axId val="1598480672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1625667264"/>
+        <c:axId val="1598816496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1265,12 +1205,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1600031648"/>
+        <c:crossAx val="1598480672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1600031648"/>
+        <c:axId val="1598480672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1387,7 +1327,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1625667264"/>
+        <c:crossAx val="1598816496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1554,7 +1494,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$6</c:f>
+              <c:f>Sheet1!$E$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1589,10 +1529,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$18</c:f>
+              <c:f>Sheet1!$A$8:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>16.0</c:v>
                 </c:pt>
@@ -1622,57 +1562,45 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>8192.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16384.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>32768.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$7:$E$18</c:f>
+              <c:f>Sheet1!$E$8:$E$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0.011671</c:v>
+                  <c:v>0.011718</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.042655</c:v>
+                  <c:v>0.042581</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.183301</c:v>
+                  <c:v>0.144921</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.598628</c:v>
+                  <c:v>0.590351</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.292074</c:v>
+                  <c:v>2.074372</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.829627</c:v>
+                  <c:v>8.190905000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40.660421</c:v>
+                  <c:v>34.470656</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>141.467868</c:v>
+                  <c:v>140.438297</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>561.42419</c:v>
+                  <c:v>593.1306949999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2262.37449</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9339.606009</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40414.75878</c:v>
+                  <c:v>2421.303074</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1684,7 +1612,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$6</c:f>
+              <c:f>Sheet1!$F$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1719,10 +1647,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$18</c:f>
+              <c:f>Sheet1!$A$8:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>16.0</c:v>
                 </c:pt>
@@ -1752,57 +1680,45 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>8192.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16384.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>32768.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$7:$F$18</c:f>
+              <c:f>Sheet1!$F$8:$F$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0.011718</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0.042581</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0.144921</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0.590351</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>2.074372</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>8.190905000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>34.470656</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0</c:v>
+                  <c:v>140.438297</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0</c:v>
+                  <c:v>593.1306949999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.0</c:v>
+                  <c:v>2421.303074</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1817,11 +1733,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1627085440"/>
-        <c:axId val="1626499808"/>
+        <c:axId val="1594184192"/>
+        <c:axId val="1654544976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1627085440"/>
+        <c:axId val="1594184192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1897,6 +1813,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1933,12 +1850,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1626499808"/>
+        <c:crossAx val="1654544976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1626499808"/>
+        <c:axId val="1654544976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2056,7 +1973,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1627085440"/>
+        <c:crossAx val="1594184192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3810,15 +3727,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3840,15 +3757,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>793750</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:colOff>641350</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3870,15 +3787,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4163,465 +4080,343 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>0.6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>3</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>5</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>6</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H7" t="s">
         <v>7</v>
       </c>
-      <c r="J6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>16</v>
       </c>
-      <c r="B7">
-        <v>0.26728400000000002</v>
-      </c>
-      <c r="C7">
-        <v>3.5693999999999997E-2</v>
-      </c>
-      <c r="D7">
-        <v>0.12889300000000001</v>
-      </c>
-      <c r="E7">
-        <v>1.1671000000000001E-2</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>4.7364999999999997E-2</v>
-      </c>
-      <c r="H7">
-        <v>0.12889300000000001</v>
-      </c>
-      <c r="J7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7">
-        <v>139</v>
+      <c r="B8">
+        <v>3.7189E-2</v>
+      </c>
+      <c r="C8">
+        <v>1.8114999999999999E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.110529</v>
+      </c>
+      <c r="E8">
+        <v>1.1717999999999999E-2</v>
+      </c>
+      <c r="F8">
+        <v>1.1717999999999999E-2</v>
+      </c>
+      <c r="G8">
+        <v>2.9832999999999998E-2</v>
+      </c>
+      <c r="H8">
+        <v>0.12224699999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>32</v>
       </c>
-      <c r="B8">
-        <v>4.8294999999999998E-2</v>
-      </c>
-      <c r="C8">
-        <v>4.2312000000000002E-2</v>
-      </c>
-      <c r="D8">
-        <v>8.6396000000000001E-2</v>
-      </c>
-      <c r="E8">
-        <v>4.2654999999999998E-2</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>8.4967000000000001E-2</v>
-      </c>
-      <c r="H8">
-        <v>8.6396000000000001E-2</v>
-      </c>
-      <c r="J8" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8">
-        <v>433</v>
+      <c r="B9">
+        <v>4.1373E-2</v>
+      </c>
+      <c r="C9">
+        <v>9.1718999999999995E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.123476</v>
+      </c>
+      <c r="E9">
+        <v>4.2581000000000001E-2</v>
+      </c>
+      <c r="F9">
+        <v>4.2581000000000001E-2</v>
+      </c>
+      <c r="G9">
+        <v>0.1343</v>
+      </c>
+      <c r="H9">
+        <v>0.16605700000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>64</v>
       </c>
-      <c r="B9">
-        <v>0.12297</v>
-      </c>
-      <c r="C9">
-        <v>0.31650800000000001</v>
-      </c>
-      <c r="D9">
-        <v>0.31263999999999997</v>
-      </c>
-      <c r="E9">
-        <v>0.18330099999999999</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0.499809</v>
-      </c>
-      <c r="H9">
-        <v>0.31263999999999997</v>
-      </c>
-      <c r="J9" t="s">
-        <v>10</v>
-      </c>
-      <c r="K9">
-        <v>2177</v>
+      <c r="B10">
+        <v>8.8540999999999995E-2</v>
+      </c>
+      <c r="C10">
+        <v>0.22778100000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.20985100000000001</v>
+      </c>
+      <c r="E10">
+        <v>0.14492099999999999</v>
+      </c>
+      <c r="F10">
+        <v>0.14492099999999999</v>
+      </c>
+      <c r="G10">
+        <v>0.37270199999999998</v>
+      </c>
+      <c r="H10">
+        <v>0.35477199999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>128</v>
       </c>
-      <c r="B10">
-        <v>0.22558600000000001</v>
-      </c>
-      <c r="C10">
-        <v>0.27678900000000001</v>
-      </c>
-      <c r="D10">
-        <v>0.31318099999999999</v>
-      </c>
-      <c r="E10">
-        <v>0.59862800000000005</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0.875417</v>
-      </c>
-      <c r="H10">
-        <v>0.31318099999999999</v>
-      </c>
-      <c r="J10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10">
-        <v>3887</v>
+      <c r="B11">
+        <v>0.23580899999999999</v>
+      </c>
+      <c r="C11">
+        <v>0.53934199999999999</v>
+      </c>
+      <c r="D11">
+        <v>0.53109399999999996</v>
+      </c>
+      <c r="E11">
+        <v>0.59035099999999996</v>
+      </c>
+      <c r="F11">
+        <v>0.59035099999999996</v>
+      </c>
+      <c r="G11">
+        <v>1.1296930000000001</v>
+      </c>
+      <c r="H11">
+        <v>1.121445</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>256</v>
       </c>
-      <c r="B11">
-        <v>0.63269900000000001</v>
-      </c>
-      <c r="C11">
-        <v>2.4634800000000001</v>
-      </c>
-      <c r="D11">
-        <v>3.9257249999999999</v>
-      </c>
-      <c r="E11">
-        <v>2.2920739999999999</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>4.7555540000000001</v>
-      </c>
-      <c r="H11">
-        <v>3.9257249999999999</v>
-      </c>
-      <c r="J11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11">
-        <v>24745</v>
+      <c r="B12">
+        <v>0.74601099999999998</v>
+      </c>
+      <c r="C12">
+        <v>1.745716</v>
+      </c>
+      <c r="D12">
+        <v>1.996095</v>
+      </c>
+      <c r="E12">
+        <v>2.0743719999999999</v>
+      </c>
+      <c r="F12">
+        <v>2.0743719999999999</v>
+      </c>
+      <c r="G12">
+        <v>3.8200880000000002</v>
+      </c>
+      <c r="H12">
+        <v>4.0704659999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>512</v>
       </c>
-      <c r="B12">
-        <v>2.4137849999999998</v>
-      </c>
-      <c r="C12">
-        <v>9.9982030000000002</v>
-      </c>
-      <c r="D12">
-        <v>6.1722789999999996</v>
-      </c>
-      <c r="E12">
-        <v>7.8296270000000003</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>17.827829999999999</v>
-      </c>
-      <c r="H12">
-        <v>6.1722789999999996</v>
-      </c>
-      <c r="J12" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12">
-        <v>125539</v>
+      <c r="B13">
+        <v>2.3754979999999999</v>
+      </c>
+      <c r="C13">
+        <v>7.5390050000000004</v>
+      </c>
+      <c r="D13">
+        <v>11.299106999999999</v>
+      </c>
+      <c r="E13">
+        <v>8.1909050000000008</v>
+      </c>
+      <c r="F13">
+        <v>8.1909050000000008</v>
+      </c>
+      <c r="G13">
+        <v>15.729908999999999</v>
+      </c>
+      <c r="H13">
+        <v>19.490010999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>1024</v>
       </c>
-      <c r="B13">
-        <v>8.2959110000000003</v>
-      </c>
-      <c r="C13">
-        <v>22.627317999999999</v>
-      </c>
-      <c r="D13">
-        <v>22.221876999999999</v>
-      </c>
-      <c r="E13">
-        <v>40.660420999999999</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>63.287739000000002</v>
-      </c>
-      <c r="H13">
-        <v>22.221876999999999</v>
-      </c>
-      <c r="J13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13">
-        <v>430119</v>
+      <c r="B14">
+        <v>9.2888009999999994</v>
+      </c>
+      <c r="C14">
+        <v>30.838740000000001</v>
+      </c>
+      <c r="D14">
+        <v>77.448294000000004</v>
+      </c>
+      <c r="E14">
+        <v>34.470655999999998</v>
+      </c>
+      <c r="F14">
+        <v>34.470655999999998</v>
+      </c>
+      <c r="G14">
+        <v>65.309396000000007</v>
+      </c>
+      <c r="H14">
+        <v>111.91895100000001</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>2048</v>
       </c>
-      <c r="B14">
-        <v>31.438592</v>
-      </c>
-      <c r="C14">
-        <v>80.662372000000005</v>
-      </c>
-      <c r="D14">
-        <v>75.349418</v>
-      </c>
-      <c r="E14">
-        <v>141.46786800000001</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>222.13023999999999</v>
-      </c>
-      <c r="H14">
-        <v>75.349418</v>
-      </c>
-      <c r="J14" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14">
-        <v>1843887</v>
+      <c r="B15">
+        <v>35.069363000000003</v>
+      </c>
+      <c r="C15">
+        <v>104.765969</v>
+      </c>
+      <c r="D15">
+        <v>301.09259200000002</v>
+      </c>
+      <c r="E15">
+        <v>140.43829700000001</v>
+      </c>
+      <c r="F15">
+        <v>140.43829700000001</v>
+      </c>
+      <c r="G15">
+        <v>245.20426499999999</v>
+      </c>
+      <c r="H15">
+        <v>441.530889</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>4096</v>
       </c>
-      <c r="B15">
-        <v>129.57210699999999</v>
-      </c>
-      <c r="C15">
-        <v>184.23211599999999</v>
-      </c>
-      <c r="D15">
-        <v>80.169452000000007</v>
-      </c>
-      <c r="E15">
-        <v>561.42418999999995</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>745.65630599999997</v>
-      </c>
-      <c r="H15">
-        <v>80.169452000000007</v>
-      </c>
-      <c r="J15" t="s">
-        <v>10</v>
-      </c>
-      <c r="K15">
-        <v>7566564</v>
+      <c r="B16">
+        <v>137.974862</v>
+      </c>
+      <c r="C16">
+        <v>228.42369500000001</v>
+      </c>
+      <c r="D16">
+        <v>170.827136</v>
+      </c>
+      <c r="E16">
+        <v>593.13069499999995</v>
+      </c>
+      <c r="F16">
+        <v>593.13069499999995</v>
+      </c>
+      <c r="G16">
+        <v>821.55439000000001</v>
+      </c>
+      <c r="H16">
+        <v>763.95783100000006</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>8192</v>
       </c>
-      <c r="B16">
-        <v>548.18113200000005</v>
-      </c>
-      <c r="C16">
-        <v>834.25004899999999</v>
-      </c>
-      <c r="D16">
-        <v>687.68384200000003</v>
-      </c>
-      <c r="E16">
-        <v>2262.3744900000002</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>3096.6245389999999</v>
-      </c>
-      <c r="H16">
-        <v>687.68384200000003</v>
-      </c>
-      <c r="J16" t="s">
-        <v>10</v>
-      </c>
-      <c r="K16">
-        <v>28011244</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>16384</v>
-      </c>
       <c r="B17">
-        <v>2023.6396030000001</v>
+        <v>526.32718999999997</v>
       </c>
       <c r="C17">
-        <v>1696.4327029999999</v>
+        <v>718.45933400000001</v>
       </c>
       <c r="D17">
-        <v>1174.4391639999999</v>
+        <v>517.91763900000001</v>
       </c>
       <c r="E17">
-        <v>9339.6060089999992</v>
+        <v>2421.3030739999999</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>2421.3030739999999</v>
       </c>
       <c r="G17">
-        <v>11036.038710000001</v>
+        <v>3139.7624080000001</v>
       </c>
       <c r="H17">
-        <v>1174.4391639999999</v>
-      </c>
-      <c r="J17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K17">
-        <v>116216126</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>32768</v>
-      </c>
-      <c r="B18">
-        <v>8251.3828250000006</v>
-      </c>
-      <c r="C18">
-        <v>3594.2870480000001</v>
-      </c>
-      <c r="D18">
-        <v>2985.5234879999998</v>
-      </c>
-      <c r="E18">
-        <v>40414.758779999996</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>44009.045819999999</v>
-      </c>
-      <c r="H18">
-        <v>2985.5234879999998</v>
-      </c>
-      <c r="J18" t="s">
-        <v>10</v>
-      </c>
-      <c r="K18">
-        <v>463642733</v>
+        <v>2939.2207130000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>